<commit_message>
Finalized the project plan
</commit_message>
<xml_diff>
--- a/Documentation/ProjectDocumentation/Project_plan.xlsx
+++ b/Documentation/ProjectDocumentation/Project_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andi\Documents\FH Hagenberg Semester 2\PRO\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B176A14E-D935-4997-8526-8DFF7CA3D136}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F10AADC-CC4D-4C32-9BB4-E369C5BB1AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Wählen Sie rechts einen Zeitraum zum Hervorheben aus.  Es folgt eine Legende, die das Diagramm beschreibt.</t>
   </si>
@@ -1002,6 +1002,51 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="41" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="42" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="43" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="44" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1013,51 +1058,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="41" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="42" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="43" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="44" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1510,20 +1510,20 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="48" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="50" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" customWidth="1"/>
-    <col min="2" max="2" width="15.58203125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="17.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="17.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="25" style="4" customWidth="1"/>
     <col min="8" max="27" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
@@ -1533,14 +1533,14 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1548,73 +1548,73 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
       <c r="Q2" s="17"/>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
       <c r="X2" s="18"/>
-      <c r="Y2" s="22" t="s">
+      <c r="Y2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
       <c r="AE2" s="19"/>
-      <c r="AF2" s="22" t="s">
+      <c r="AF2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
       <c r="AO2" s="20"/>
-      <c r="AP2" s="22" t="s">
+      <c r="AP2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="23"/>
-      <c r="AR2" s="23"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="23"/>
-      <c r="AY2" s="23"/>
-      <c r="AZ2" s="23"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="38"/>
+      <c r="AY2" s="38"/>
+      <c r="AZ2" s="38"/>
+    </row>
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="36" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="31" t="s">
@@ -1643,13 +1643,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="28"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="35"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1831,8 +1831,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="32" t="s">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="7">
@@ -1848,11 +1848,11 @@
         <v>4</v>
       </c>
       <c r="G5" s="8">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="7">
@@ -1871,8 +1871,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="33" t="s">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7">
@@ -1891,8 +1891,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="7">
@@ -1904,35 +1904,35 @@
       <c r="E8" s="7">
         <v>4</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="30">
         <v>1</v>
       </c>
       <c r="G8" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="47.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="47.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
       </c>
       <c r="D9" s="7">
-        <v>9</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="30">
+        <v>2</v>
+      </c>
+      <c r="F9" s="30">
+        <v>7</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="25" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="7">
@@ -1951,8 +1951,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="35" t="s">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="25" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="7">
@@ -1961,18 +1961,18 @@
       <c r="D11" s="7">
         <v>3</v>
       </c>
-      <c r="E11" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>32</v>
+      <c r="E11" s="30">
+        <v>5</v>
+      </c>
+      <c r="F11" s="30">
+        <v>2</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="25" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="7">
@@ -1981,18 +1981,18 @@
       <c r="D12" s="7">
         <v>4</v>
       </c>
-      <c r="E12" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>32</v>
+      <c r="E12" s="30">
+        <v>7</v>
+      </c>
+      <c r="F12" s="30">
+        <v>2</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="7">
@@ -2001,18 +2001,18 @@
       <c r="D13" s="7">
         <v>1</v>
       </c>
-      <c r="E13" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>32</v>
+      <c r="E13" s="30">
+        <v>8</v>
+      </c>
+      <c r="F13" s="30">
+        <v>1</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="35.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="7">
@@ -2021,18 +2021,18 @@
       <c r="D14" s="7">
         <v>2</v>
       </c>
-      <c r="E14" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>32</v>
+      <c r="E14" s="30">
+        <v>9</v>
+      </c>
+      <c r="F14" s="30">
+        <v>4</v>
       </c>
       <c r="G14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="9">
@@ -2041,18 +2041,18 @@
       <c r="D15" s="7">
         <v>1</v>
       </c>
-      <c r="E15" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>32</v>
+      <c r="E15" s="30">
+        <v>11</v>
+      </c>
+      <c r="F15" s="30">
+        <v>1</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="7">
@@ -2061,18 +2061,18 @@
       <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>32</v>
+      <c r="E16" s="30">
+        <v>11</v>
+      </c>
+      <c r="F16" s="30">
+        <v>1</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="7">
@@ -2081,18 +2081,18 @@
       <c r="D17" s="7">
         <v>1</v>
       </c>
-      <c r="E17" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="40" t="s">
-        <v>32</v>
+      <c r="E17" s="30">
+        <v>8</v>
+      </c>
+      <c r="F17" s="30">
+        <v>1</v>
       </c>
       <c r="G17" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="7">
@@ -2101,18 +2101,18 @@
       <c r="D18" s="7">
         <v>1</v>
       </c>
-      <c r="E18" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="40" t="s">
-        <v>32</v>
+      <c r="E18" s="30">
+        <v>9</v>
+      </c>
+      <c r="F18" s="30">
+        <v>2</v>
       </c>
       <c r="G18" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="28" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="7">
@@ -2121,18 +2121,18 @@
       <c r="D19" s="7">
         <v>2</v>
       </c>
-      <c r="E19" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="40" t="s">
-        <v>32</v>
+      <c r="E19" s="30">
+        <v>11</v>
+      </c>
+      <c r="F19" s="30">
+        <v>2</v>
       </c>
       <c r="G19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="7">
@@ -2141,18 +2141,18 @@
       <c r="D20" s="7">
         <v>1</v>
       </c>
-      <c r="E20" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="40" t="s">
-        <v>32</v>
+      <c r="E20" s="30">
+        <v>11</v>
+      </c>
+      <c r="F20" s="30">
+        <v>1</v>
       </c>
       <c r="G20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="7">
@@ -2161,17 +2161,17 @@
       <c r="D21" s="7">
         <v>1</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="30">
+        <v>12</v>
+      </c>
+      <c r="F21" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="40" t="s">
-        <v>32</v>
-      </c>
       <c r="G21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -2179,7 +2179,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -2187,7 +2187,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -2195,7 +2195,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -2203,7 +2203,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -2211,7 +2211,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -2219,7 +2219,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -2227,7 +2227,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -2235,7 +2235,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -2245,6 +2245,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AP2:AZ2"/>
+    <mergeCell ref="AF2:AN2"/>
+    <mergeCell ref="Y2:AD2"/>
+    <mergeCell ref="R2:W2"/>
+    <mergeCell ref="K2:P2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
@@ -2252,11 +2257,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="AP2:AZ2"/>
-    <mergeCell ref="AF2:AN2"/>
-    <mergeCell ref="Y2:AD2"/>
-    <mergeCell ref="R2:W2"/>
-    <mergeCell ref="K2:P2"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>